<commit_message>
Reupload to sync changes
</commit_message>
<xml_diff>
--- a/server/DummyCSV/accountStatuses.xlsx
+++ b/server/DummyCSV/accountStatuses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonng/Desktop/booKING-main/server/DummyCSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC22C603-FF05-C940-AA9B-587D7F1BB92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36067FB3-E86A-324F-98CB-7DDCB3FD2059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{67662717-BC5A-9B45-9D1B-C292D966A6AC}"/>
   </bookViews>
@@ -45,16 +45,16 @@
     <t>statusDescription</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Normal account</t>
-  </si>
-  <si>
-    <t>Banned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Due to malicious activities by user </t>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Offline</t>
+  </si>
+  <si>
+    <t>Currently logged in.</t>
+  </si>
+  <si>
+    <t>Currently not logged in.</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,7 +438,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -446,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>